<commit_message>
doc(journal de travail): rédaction du journal de travail avec les tâches effectuées
</commit_message>
<xml_diff>
--- a/JDT/T-P_FUN-MatiasDenis-JDT.xlsx
+++ b/JDT/T-P_FUN-MatiasDenis-JDT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_FUN\P_FUN\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DC310B-E0C2-4637-A8DC-E5538A0F8A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE2F2EE-279E-4CDD-9A1F-9EE130C07243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="56">
   <si>
     <t>Module :</t>
   </si>
@@ -191,13 +191,7 @@
     <t>Création maquette Figma</t>
   </si>
   <si>
-    <t>Création de la maquette de l'interface graphique sur Figma.</t>
-  </si>
-  <si>
     <t>Ebauche de rapport de projet</t>
-  </si>
-  <si>
-    <t>Un début de rapport de projet a été créé en suivant les demandes du cahier des charges.</t>
   </si>
   <si>
     <t>Accident.</t>
@@ -218,6 +212,35 @@
   </si>
   <si>
     <t>Congé - lundi du jeûne.</t>
+  </si>
+  <si>
+    <t>Correction d'un bug d'import de csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programmation assistée </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScottPlot - Interactive Plotting Library for .NET
+chatgpt.com
+https://learn.microsoft.com/fr-fr/visualstudio/ide/create-csharp-winform-visual-studio?view=vs-2022 
+</t>
+  </si>
+  <si>
+    <t>Rédaction suite du rapport de projet</t>
+  </si>
+  <si>
+    <t>Programmation assistée à l'aide de l'IA ainsi que de la documentation microsoft. Etant données les tâches à faire et la durée du projet, il est très compliqué d'apprendre le C# en Windows Forms et de faire un projet de A à Z sans une aide externe. // tâches en cours, finies etc...</t>
+  </si>
+  <si>
+    <t>Création de la maquette de l'interface graphique sur Figma. Tâche terminée.</t>
+  </si>
+  <si>
+    <t>Un début de rapport de projet a été créé en suivant les demandes du cahier des charges. Tâche en cours: la structure de base a été créée et certains points ont été rédigés comme l'introduction, les objectifs de jeu, le domaine d'application et la planification.</t>
+  </si>
+  <si>
+    <t>Rédaction de ce qui a été effectué jusqu'à maintenant dans le projet. 
+Tâche en cours: rédaction des points objectifs pédagogiques, production, usage de l'IA.
+Tâches finies: la structure de base, l'introduction, les objectifs de jeu, le domaine d'application et la planification.</t>
   </si>
 </sst>
 </file>
@@ -857,7 +880,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1127,6 +1150,9 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1778,8 +1804,8 @@
   </sheetPr>
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2088,7 +2114,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="60"/>
       <c r="E26" s="60"/>
@@ -2101,7 +2127,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="71" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27" s="60"/>
       <c r="E27" s="60"/>
@@ -2113,7 +2139,9 @@
       <c r="B28" s="80">
         <v>8</v>
       </c>
-      <c r="C28" s="72"/>
+      <c r="C28" s="72" t="s">
+        <v>49</v>
+      </c>
       <c r="D28" s="60"/>
       <c r="E28" s="60"/>
       <c r="F28" s="60"/>
@@ -2124,7 +2152,9 @@
       <c r="B29" s="82">
         <v>9</v>
       </c>
-      <c r="C29" s="72"/>
+      <c r="C29" s="72" t="s">
+        <v>48</v>
+      </c>
       <c r="D29" s="60"/>
       <c r="E29" s="60"/>
       <c r="F29" s="60"/>
@@ -2135,7 +2165,9 @@
       <c r="B30" s="80">
         <v>10</v>
       </c>
-      <c r="C30" s="71"/>
+      <c r="C30" s="71" t="s">
+        <v>51</v>
+      </c>
       <c r="D30" s="60"/>
       <c r="E30" s="60"/>
       <c r="F30" s="60"/>
@@ -2834,27 +2866,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2884,27 +2916,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -3755,8 +3787,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:I153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3764,7 +3796,7 @@
     <col min="1" max="1" width="21.42578125" style="29" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" style="29" customWidth="1"/>
     <col min="3" max="3" width="87" style="29" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" style="29" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="29"/>
   </cols>
   <sheetData>
@@ -3971,21 +4003,21 @@
         <v>7</v>
       </c>
       <c r="C22" s="90" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="B23" s="2">
         <v>2</v>
       </c>
       <c r="C23" s="91" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D23" s="10"/>
     </row>
@@ -4203,7 +4235,7 @@
         <v>9</v>
       </c>
       <c r="C41" s="90" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D41" s="9"/>
     </row>
@@ -4341,16 +4373,16 @@
     </row>
     <row r="60" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B60" s="4">
         <v>9</v>
       </c>
       <c r="C60" s="90" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D60" s="92" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4493,7 +4525,7 @@
         <v>9</v>
       </c>
       <c r="C79" s="90" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D79" s="9"/>
     </row>
@@ -4629,16 +4661,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="10"/>
+    <row r="98" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B98" s="4">
+        <v>5</v>
+      </c>
+      <c r="C98" s="90" t="s">
+        <v>52</v>
+      </c>
+      <c r="D98" s="97" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B99" s="2">
+        <v>4</v>
+      </c>
+      <c r="C99" s="91" t="s">
+        <v>55</v>
+      </c>
       <c r="D99" s="10"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4725,7 +4771,7 @@
       </c>
       <c r="B113" s="48">
         <f>SUM(B98:B112)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C113" s="89" t="s">
         <v>28</v>
@@ -5038,16 +5084,17 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D60" r:id="rId1" xr:uid="{525590D3-AE3F-412E-AE63-77E2FB54C37E}"/>
+    <hyperlink ref="D98" r:id="rId2" display="https://scottplot.net/" xr:uid="{96953D07-F238-4D18-B372-BC8B3B97A872}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId5" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+        <control shapeId="43009" r:id="rId6" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5066,7 +5113,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId5" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId6" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5303,6 +5350,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
@@ -5311,15 +5367,6 @@
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5342,6 +5389,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5350,12 +5405,4 @@
     <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(journal de travail): journal de travail à jour avec les prompts chatgpt
</commit_message>
<xml_diff>
--- a/JDT/T-P_FUN-MatiasDenis-JDT.xlsx
+++ b/JDT/T-P_FUN-MatiasDenis-JDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_FUN\P_FUN\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0A0B7D-F2F1-47C9-9B96-CE2B60054FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31D15B5-8D49-46D4-ACF4-AD6E792265BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
   <si>
     <t>Module :</t>
   </si>
@@ -200,12 +200,6 @@
     <t xml:space="preserve">Programmation assistée </t>
   </si>
   <si>
-    <t xml:space="preserve">ScottPlot - Interactive Plotting Library for .NET
-chatgpt.com
-https://learn.microsoft.com/fr-fr/visualstudio/ide/create-csharp-winform-visual-studio?view=vs-2022 
-</t>
-  </si>
-  <si>
     <t>Rédaction suite du rapport de projet</t>
   </si>
   <si>
@@ -272,6 +266,12 @@
     <t>Tâche 10: Rédiger la suite du rapport de projet
 Les parties sur les objectifs pédagogiques et les tests fonctionnels sont rédigées.
 Tâche en cours.</t>
+  </si>
+  <si>
+    <t>ScottPlot - Interactive Plotting Library for .NET
+chatgpt.com
+https://learn.microsoft.com/fr-fr/visualstudio/ide/create-csharp-winform-visual-studio?view=vs-2022 
+https://chatgpt.com/c/68c7f767-915c-832b-bc1e-3d01b5980f03</t>
   </si>
 </sst>
 </file>
@@ -911,21 +911,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -933,138 +933,137 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="3" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="3" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1080,23 +1079,23 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1107,7 +1106,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1122,10 +1121,10 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1133,17 +1132,16 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="15" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1151,19 +1149,19 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1174,17 +1172,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1557,7 +1559,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
+          <xdr:colOff>259080</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -1837,7 +1839,7 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M73"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
@@ -1845,1043 +1847,614 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="58" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" style="58" customWidth="1"/>
-    <col min="3" max="3" width="88.5703125" style="58" customWidth="1"/>
-    <col min="4" max="4" width="3.42578125" style="58" customWidth="1"/>
-    <col min="5" max="6" width="11.5703125" style="58"/>
-    <col min="7" max="7" width="3.28515625" style="58" customWidth="1"/>
-    <col min="8" max="16384" width="11.5703125" style="58"/>
+    <col min="1" max="1" width="16.5703125" style="57" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" style="57" customWidth="1"/>
+    <col min="3" max="3" width="88.5703125" style="57" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" style="57" customWidth="1"/>
+    <col min="5" max="6" width="11.5703125" style="57"/>
+    <col min="7" max="7" width="3.28515625" style="57" customWidth="1"/>
+    <col min="8" max="16384" width="11.5703125" style="57"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="55"/>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="57"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
     </row>
     <row r="2" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="61"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="60"/>
     </row>
     <row r="3" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="59"/>
-      <c r="B3" s="62" t="s">
+      <c r="A3" s="58"/>
+      <c r="B3" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="60"/>
     </row>
     <row r="4" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="64" t="s">
+      <c r="A4" s="58"/>
+      <c r="B4" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="60"/>
     </row>
     <row r="5" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="59"/>
-      <c r="B5" s="64" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="61"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="60"/>
     </row>
     <row r="6" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="59"/>
-      <c r="B6" s="66" t="s">
+      <c r="A6" s="58"/>
+      <c r="B6" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="67" t="s">
+      <c r="C6" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="60"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="59"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="61"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="60"/>
     </row>
     <row r="8" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="61"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="60"/>
     </row>
     <row r="9" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="59"/>
-      <c r="B9" s="62" t="s">
+      <c r="A9" s="58"/>
+      <c r="B9" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="67">
         <v>45894</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
     </row>
     <row r="10" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="59"/>
-      <c r="B10" s="69" t="s">
+      <c r="A10" s="58"/>
+      <c r="B10" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="70">
+      <c r="C10" s="69">
         <v>45957</v>
       </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="61"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
     </row>
     <row r="11" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="59"/>
-      <c r="B11" s="69" t="s">
+      <c r="A11" s="58"/>
+      <c r="B11" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="71">
+      <c r="C11" s="70">
         <v>8</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="61"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
     </row>
     <row r="12" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="59"/>
-      <c r="B12" s="64" t="s">
+      <c r="A12" s="58"/>
+      <c r="B12" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="72">
+      <c r="C12" s="71">
         <v>3</v>
       </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="61"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
     </row>
     <row r="13" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="64" t="s">
+      <c r="A13" s="58"/>
+      <c r="B13" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="72">
+      <c r="C13" s="71">
         <v>3</v>
       </c>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="61"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
     </row>
     <row r="14" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="59"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="74" t="s">
+      <c r="A14" s="58"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="61"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="61"/>
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
     </row>
     <row r="16" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="75"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="77"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="78"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-    </row>
-    <row r="18" spans="1:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="79"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="61"/>
-    </row>
-    <row r="19" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="79"/>
-      <c r="B19" s="94" t="s">
+      <c r="A16" s="74"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="76"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="77"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="78"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
+    </row>
+    <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="78"/>
+      <c r="B19" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="95"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="61"/>
-    </row>
-    <row r="20" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="79"/>
-      <c r="B20" s="80" t="s">
+      <c r="C19" s="94"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="60"/>
+    </row>
+    <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="78"/>
+      <c r="B20" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="81" t="s">
+      <c r="C20" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="61"/>
-    </row>
-    <row r="21" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="79"/>
-      <c r="B21" s="80">
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
+    </row>
+    <row r="21" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="78"/>
+      <c r="B21" s="79">
         <v>1</v>
       </c>
-      <c r="C21" s="70" t="s">
+      <c r="C21" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="61"/>
-    </row>
-    <row r="22" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="79"/>
-      <c r="B22" s="80">
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="60"/>
+    </row>
+    <row r="22" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="78"/>
+      <c r="B22" s="79">
         <v>2</v>
       </c>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="61"/>
-    </row>
-    <row r="23" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="79"/>
-      <c r="B23" s="82">
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
+    </row>
+    <row r="23" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="78"/>
+      <c r="B23" s="81">
         <v>3</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="61"/>
-    </row>
-    <row r="24" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="79"/>
-      <c r="B24" s="80">
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="60"/>
+    </row>
+    <row r="24" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="78"/>
+      <c r="B24" s="79">
         <v>4</v>
       </c>
-      <c r="C24" s="71" t="s">
+      <c r="C24" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="61"/>
-    </row>
-    <row r="25" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="79"/>
-      <c r="B25" s="80">
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="60"/>
+    </row>
+    <row r="25" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="78"/>
+      <c r="B25" s="79">
         <v>5</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="61"/>
-    </row>
-    <row r="26" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="79"/>
-      <c r="B26" s="82">
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+    </row>
+    <row r="26" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="78"/>
+      <c r="B26" s="81">
         <v>6</v>
       </c>
-      <c r="C26" s="71" t="s">
+      <c r="C26" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="61"/>
-    </row>
-    <row r="27" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="79"/>
-      <c r="B27" s="80">
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="60"/>
+    </row>
+    <row r="27" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="78"/>
+      <c r="B27" s="79">
         <v>7</v>
       </c>
-      <c r="C27" s="71" t="s">
+      <c r="C27" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="61"/>
-    </row>
-    <row r="28" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="79"/>
-      <c r="B28" s="80">
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="60"/>
+    </row>
+    <row r="28" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="78"/>
+      <c r="B28" s="79">
         <v>8</v>
       </c>
-      <c r="C28" s="72" t="s">
+      <c r="C28" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="61"/>
-    </row>
-    <row r="29" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="79"/>
-      <c r="B29" s="82">
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="60"/>
+    </row>
+    <row r="29" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="78"/>
+      <c r="B29" s="81">
         <v>9</v>
       </c>
-      <c r="C29" s="72" t="s">
+      <c r="C29" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="61"/>
-    </row>
-    <row r="30" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="79"/>
-      <c r="B30" s="80">
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="60"/>
+    </row>
+    <row r="30" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="78"/>
+      <c r="B30" s="79">
         <v>10</v>
       </c>
-      <c r="C30" s="71" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
-    </row>
-    <row r="31" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="79"/>
-      <c r="B31" s="80">
+      <c r="C30" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="60"/>
+    </row>
+    <row r="31" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="78"/>
+      <c r="B31" s="79">
         <v>11</v>
       </c>
-      <c r="C31" s="71"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="83"/>
-      <c r="J31" s="83"/>
-      <c r="K31" s="83"/>
-      <c r="L31" s="83"/>
-      <c r="M31" s="83"/>
-    </row>
-    <row r="32" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="79"/>
-      <c r="B32" s="82">
+      <c r="C31" s="70"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="60"/>
+    </row>
+    <row r="32" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="78"/>
+      <c r="B32" s="81">
         <v>12</v>
       </c>
-      <c r="C32" s="71"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="83"/>
-      <c r="J32" s="83"/>
-      <c r="K32" s="83"/>
-      <c r="L32" s="83"/>
-      <c r="M32" s="83"/>
-    </row>
-    <row r="33" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="79"/>
-      <c r="B33" s="80">
+      <c r="C32" s="70"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="60"/>
+    </row>
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="78"/>
+      <c r="B33" s="79">
         <v>13</v>
       </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="83"/>
-      <c r="I33" s="83"/>
-      <c r="J33" s="83"/>
-      <c r="K33" s="83"/>
-      <c r="L33" s="83"/>
-      <c r="M33" s="83"/>
-    </row>
-    <row r="34" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="79"/>
-      <c r="B34" s="80">
+      <c r="C33" s="70"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
+    </row>
+    <row r="34" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="78"/>
+      <c r="B34" s="79">
         <v>14</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="83"/>
-      <c r="I34" s="83"/>
-      <c r="J34" s="83"/>
-      <c r="K34" s="83"/>
-      <c r="L34" s="83"/>
-      <c r="M34" s="83"/>
-    </row>
-    <row r="35" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="79"/>
-      <c r="B35" s="82">
+      <c r="C34" s="71"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="60"/>
+    </row>
+    <row r="35" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="78"/>
+      <c r="B35" s="81">
         <v>15</v>
       </c>
-      <c r="C35" s="72"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
-      <c r="J35" s="83"/>
-      <c r="K35" s="83"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="83"/>
-    </row>
-    <row r="36" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="79"/>
-      <c r="B36" s="80">
+      <c r="C35" s="71"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="60"/>
+    </row>
+    <row r="36" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="78"/>
+      <c r="B36" s="79">
         <v>16</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="83"/>
-      <c r="M36" s="83"/>
-    </row>
-    <row r="37" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="79"/>
-      <c r="B37" s="80">
+      <c r="C36" s="70"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="59"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="60"/>
+    </row>
+    <row r="37" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="78"/>
+      <c r="B37" s="79">
         <v>17</v>
       </c>
-      <c r="C37" s="71"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="61"/>
-      <c r="H37" s="83"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="83"/>
-      <c r="M37" s="83"/>
-    </row>
-    <row r="38" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="79"/>
-      <c r="B38" s="82">
+      <c r="C37" s="70"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="60"/>
+    </row>
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="78"/>
+      <c r="B38" s="81">
         <v>18</v>
       </c>
-      <c r="C38" s="71"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="83"/>
-      <c r="I38" s="83"/>
-      <c r="J38" s="83"/>
-      <c r="K38" s="83"/>
-      <c r="L38" s="83"/>
-      <c r="M38" s="83"/>
-    </row>
-    <row r="39" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="79"/>
-      <c r="B39" s="80">
+      <c r="C38" s="70"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="60"/>
+    </row>
+    <row r="39" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="78"/>
+      <c r="B39" s="79">
         <v>19</v>
       </c>
-      <c r="C39" s="71"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="83"/>
-      <c r="I39" s="83"/>
-      <c r="J39" s="83"/>
-      <c r="K39" s="83"/>
-      <c r="L39" s="83"/>
-      <c r="M39" s="83"/>
-    </row>
-    <row r="40" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="79"/>
-      <c r="B40" s="80">
+      <c r="C39" s="70"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="60"/>
+    </row>
+    <row r="40" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="78"/>
+      <c r="B40" s="79">
         <v>20</v>
       </c>
-      <c r="C40" s="72"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="83"/>
-      <c r="I40" s="83"/>
-      <c r="J40" s="83"/>
-      <c r="K40" s="83"/>
-      <c r="L40" s="83"/>
-      <c r="M40" s="83"/>
-    </row>
-    <row r="41" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="79"/>
-      <c r="B41" s="82">
+      <c r="C40" s="71"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="60"/>
+    </row>
+    <row r="41" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="78"/>
+      <c r="B41" s="81">
         <v>21</v>
       </c>
-      <c r="C41" s="72"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="83"/>
-      <c r="I41" s="83"/>
-      <c r="J41" s="83"/>
-      <c r="K41" s="83"/>
-      <c r="L41" s="83"/>
-      <c r="M41" s="83"/>
-    </row>
-    <row r="42" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="79"/>
-      <c r="B42" s="80">
+      <c r="C41" s="71"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="60"/>
+    </row>
+    <row r="42" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="78"/>
+      <c r="B42" s="79">
         <v>22</v>
       </c>
-      <c r="C42" s="71"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="83"/>
-      <c r="I42" s="83"/>
-      <c r="J42" s="83"/>
-      <c r="K42" s="83"/>
-      <c r="L42" s="83"/>
-      <c r="M42" s="83"/>
-    </row>
-    <row r="43" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="79"/>
-      <c r="B43" s="80">
+      <c r="C42" s="70"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="60"/>
+    </row>
+    <row r="43" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="78"/>
+      <c r="B43" s="79">
         <v>23</v>
       </c>
-      <c r="C43" s="71"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="83"/>
-      <c r="I43" s="83"/>
-      <c r="J43" s="83"/>
-      <c r="K43" s="83"/>
-      <c r="L43" s="83"/>
-      <c r="M43" s="83"/>
-    </row>
-    <row r="44" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="79"/>
-      <c r="B44" s="82">
+      <c r="C43" s="70"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="60"/>
+    </row>
+    <row r="44" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="78"/>
+      <c r="B44" s="81">
         <v>24</v>
       </c>
-      <c r="C44" s="71"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="83"/>
-      <c r="I44" s="83"/>
-      <c r="J44" s="83"/>
-      <c r="K44" s="83"/>
-      <c r="L44" s="83"/>
-      <c r="M44" s="83"/>
-    </row>
-    <row r="45" spans="1:13" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="79"/>
-      <c r="B45" s="84">
+      <c r="C44" s="70"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="60"/>
+    </row>
+    <row r="45" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="78"/>
+      <c r="B45" s="82">
         <v>25</v>
       </c>
-      <c r="C45" s="85"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="83"/>
-      <c r="I45" s="83"/>
-      <c r="J45" s="83"/>
-      <c r="K45" s="83"/>
-      <c r="L45" s="83"/>
-      <c r="M45" s="83"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="79"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="83"/>
-      <c r="I46" s="83"/>
-      <c r="J46" s="83"/>
-      <c r="K46" s="83"/>
-      <c r="L46" s="83"/>
-      <c r="M46" s="83"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="79"/>
-      <c r="B47" s="60"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="83"/>
-      <c r="I47" s="83"/>
-      <c r="J47" s="83"/>
-      <c r="K47" s="83"/>
-      <c r="L47" s="83"/>
-      <c r="M47" s="83"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="79"/>
-      <c r="B48" s="60"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="60"/>
-      <c r="F48" s="60"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="83"/>
-      <c r="I48" s="83"/>
-      <c r="J48" s="83"/>
-      <c r="K48" s="83"/>
-      <c r="L48" s="83"/>
-      <c r="M48" s="83"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="79"/>
-      <c r="B49" s="60"/>
-      <c r="C49" s="60"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="60"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="83"/>
-      <c r="I49" s="83"/>
-      <c r="J49" s="83"/>
-      <c r="K49" s="83"/>
-      <c r="L49" s="83"/>
-      <c r="M49" s="83"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="79"/>
-      <c r="B50" s="60"/>
-      <c r="C50" s="60"/>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="83"/>
-      <c r="I50" s="83"/>
-      <c r="J50" s="83"/>
-      <c r="K50" s="83"/>
-      <c r="L50" s="83"/>
-      <c r="M50" s="83"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="79"/>
-      <c r="B51" s="60"/>
-      <c r="C51" s="60"/>
-      <c r="D51" s="60"/>
-      <c r="E51" s="60"/>
-      <c r="F51" s="60"/>
-      <c r="G51" s="61"/>
-      <c r="H51" s="83"/>
-      <c r="I51" s="83"/>
-      <c r="J51" s="83"/>
-      <c r="K51" s="83"/>
-      <c r="L51" s="83"/>
-      <c r="M51" s="83"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="79"/>
-      <c r="B52" s="60"/>
-      <c r="C52" s="60"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="60"/>
-      <c r="F52" s="60"/>
-      <c r="G52" s="61"/>
-      <c r="H52" s="83"/>
-      <c r="I52" s="83"/>
-      <c r="J52" s="83"/>
-      <c r="K52" s="83"/>
-      <c r="L52" s="83"/>
-      <c r="M52" s="83"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="79"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="60"/>
-      <c r="F53" s="60"/>
-      <c r="G53" s="61"/>
-      <c r="H53" s="83"/>
-      <c r="I53" s="83"/>
-      <c r="J53" s="83"/>
-      <c r="K53" s="83"/>
-      <c r="L53" s="83"/>
-      <c r="M53" s="83"/>
-    </row>
-    <row r="54" spans="1:13" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="86"/>
-      <c r="B54" s="76"/>
-      <c r="C54" s="76"/>
-      <c r="D54" s="76"/>
-      <c r="E54" s="76"/>
-      <c r="F54" s="76"/>
-      <c r="G54" s="77"/>
-      <c r="H54" s="83"/>
-      <c r="I54" s="83"/>
-      <c r="J54" s="83"/>
-      <c r="K54" s="83"/>
-      <c r="L54" s="83"/>
-      <c r="M54" s="83"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="83"/>
-      <c r="B55" s="83"/>
-      <c r="C55" s="83"/>
-      <c r="D55" s="83"/>
-      <c r="E55" s="83"/>
-      <c r="F55" s="83"/>
-      <c r="G55" s="83"/>
-      <c r="H55" s="83"/>
-      <c r="I55" s="83"/>
-      <c r="J55" s="83"/>
-      <c r="K55" s="83"/>
-      <c r="L55" s="83"/>
-      <c r="M55" s="83"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="83"/>
-      <c r="B56" s="83"/>
-      <c r="C56" s="83"/>
-      <c r="D56" s="83"/>
-      <c r="E56" s="83"/>
-      <c r="F56" s="83"/>
-      <c r="G56" s="83"/>
-      <c r="H56" s="83"/>
-      <c r="I56" s="83"/>
-      <c r="J56" s="83"/>
-      <c r="K56" s="83"/>
-      <c r="L56" s="83"/>
-      <c r="M56" s="83"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="83"/>
-      <c r="B57" s="83"/>
-      <c r="C57" s="83"/>
-      <c r="D57" s="83"/>
-      <c r="E57" s="83"/>
-      <c r="F57" s="83"/>
-      <c r="G57" s="83"/>
-      <c r="H57" s="83"/>
-      <c r="I57" s="83"/>
-      <c r="J57" s="83"/>
-      <c r="K57" s="83"/>
-      <c r="L57" s="83"/>
-      <c r="M57" s="83"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="83"/>
-      <c r="B58" s="83"/>
-      <c r="C58" s="83"/>
-      <c r="D58" s="83"/>
-      <c r="E58" s="83"/>
-      <c r="F58" s="83"/>
-      <c r="G58" s="83"/>
-      <c r="H58" s="83"/>
-      <c r="I58" s="83"/>
-      <c r="J58" s="83"/>
-      <c r="K58" s="83"/>
-      <c r="L58" s="83"/>
-      <c r="M58" s="83"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="83"/>
-      <c r="B59" s="83"/>
-      <c r="C59" s="83"/>
-      <c r="D59" s="83"/>
-      <c r="E59" s="83"/>
-      <c r="F59" s="83"/>
-      <c r="G59" s="83"/>
-      <c r="H59" s="83"/>
-      <c r="I59" s="83"/>
-      <c r="J59" s="83"/>
-      <c r="K59" s="83"/>
-      <c r="L59" s="83"/>
-      <c r="M59" s="83"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="83"/>
-      <c r="B60" s="83"/>
-      <c r="C60" s="83"/>
-      <c r="D60" s="83"/>
-      <c r="E60" s="83"/>
-      <c r="F60" s="83"/>
-      <c r="G60" s="83"/>
-      <c r="H60" s="83"/>
-      <c r="I60" s="83"/>
-      <c r="J60" s="83"/>
-      <c r="K60" s="83"/>
-      <c r="L60" s="83"/>
-      <c r="M60" s="83"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="83"/>
-      <c r="B61" s="83"/>
-      <c r="C61" s="83"/>
-      <c r="D61" s="83"/>
-      <c r="E61" s="83"/>
-      <c r="F61" s="83"/>
-      <c r="G61" s="83"/>
-      <c r="H61" s="83"/>
-      <c r="I61" s="83"/>
-      <c r="J61" s="83"/>
-      <c r="K61" s="83"/>
-      <c r="L61" s="83"/>
-      <c r="M61" s="83"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="83"/>
-      <c r="B62" s="83"/>
-      <c r="C62" s="83"/>
-      <c r="D62" s="83"/>
-      <c r="E62" s="83"/>
-      <c r="F62" s="83"/>
-      <c r="G62" s="83"/>
-      <c r="H62" s="83"/>
-      <c r="I62" s="83"/>
-      <c r="J62" s="83"/>
-      <c r="K62" s="83"/>
-      <c r="L62" s="83"/>
-      <c r="M62" s="83"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="83"/>
-      <c r="B63" s="83"/>
-      <c r="C63" s="83"/>
-      <c r="D63" s="83"/>
-      <c r="E63" s="83"/>
-      <c r="F63" s="83"/>
-      <c r="G63" s="83"/>
-      <c r="H63" s="83"/>
-      <c r="I63" s="83"/>
-      <c r="J63" s="83"/>
-      <c r="K63" s="83"/>
-      <c r="L63" s="83"/>
-      <c r="M63" s="83"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="83"/>
-      <c r="B64" s="83"/>
-      <c r="C64" s="83"/>
-      <c r="D64" s="83"/>
-      <c r="E64" s="83"/>
-      <c r="F64" s="83"/>
-      <c r="G64" s="83"/>
-      <c r="H64" s="83"/>
-      <c r="I64" s="83"/>
-      <c r="J64" s="83"/>
-      <c r="K64" s="83"/>
-      <c r="L64" s="83"/>
-      <c r="M64" s="83"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A65" s="83"/>
-      <c r="B65" s="83"/>
-      <c r="C65" s="83"/>
-      <c r="D65" s="83"/>
-      <c r="E65" s="83"/>
-      <c r="F65" s="83"/>
-      <c r="G65" s="83"/>
-      <c r="H65" s="83"/>
-      <c r="I65" s="83"/>
-      <c r="J65" s="83"/>
-      <c r="K65" s="83"/>
-      <c r="L65" s="83"/>
-      <c r="M65" s="83"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="83"/>
-      <c r="B66" s="83"/>
-      <c r="C66" s="83"/>
-      <c r="D66" s="83"/>
-      <c r="E66" s="83"/>
-      <c r="F66" s="83"/>
-      <c r="G66" s="83"/>
-      <c r="H66" s="83"/>
-      <c r="I66" s="83"/>
-      <c r="J66" s="83"/>
-      <c r="K66" s="83"/>
-      <c r="L66" s="83"/>
-      <c r="M66" s="83"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="83"/>
-      <c r="B67" s="83"/>
-      <c r="C67" s="83"/>
-      <c r="D67" s="83"/>
-      <c r="E67" s="83"/>
-      <c r="F67" s="83"/>
-      <c r="G67" s="83"/>
-      <c r="H67" s="83"/>
-      <c r="I67" s="83"/>
-      <c r="J67" s="83"/>
-      <c r="K67" s="83"/>
-      <c r="L67" s="83"/>
-      <c r="M67" s="83"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="83"/>
-      <c r="B68" s="83"/>
-      <c r="C68" s="83"/>
-      <c r="D68" s="83"/>
-      <c r="E68" s="83"/>
-      <c r="F68" s="83"/>
-      <c r="G68" s="83"/>
-      <c r="H68" s="83"/>
-      <c r="I68" s="83"/>
-      <c r="J68" s="83"/>
-      <c r="K68" s="83"/>
-      <c r="L68" s="83"/>
-      <c r="M68" s="83"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="83"/>
-      <c r="B69" s="83"/>
-      <c r="C69" s="83"/>
-      <c r="D69" s="83"/>
-      <c r="E69" s="83"/>
-      <c r="F69" s="83"/>
-      <c r="G69" s="83"/>
-      <c r="H69" s="83"/>
-      <c r="I69" s="83"/>
-      <c r="J69" s="83"/>
-      <c r="K69" s="83"/>
-      <c r="L69" s="83"/>
-      <c r="M69" s="83"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A70" s="83"/>
-      <c r="B70" s="83"/>
-      <c r="C70" s="83"/>
-      <c r="D70" s="83"/>
-      <c r="E70" s="83"/>
-      <c r="F70" s="83"/>
-      <c r="G70" s="83"/>
-      <c r="H70" s="83"/>
-      <c r="I70" s="83"/>
-      <c r="J70" s="83"/>
-      <c r="K70" s="83"/>
-      <c r="L70" s="83"/>
-      <c r="M70" s="83"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A71" s="83"/>
-      <c r="B71" s="83"/>
-      <c r="C71" s="83"/>
-      <c r="D71" s="83"/>
-      <c r="E71" s="83"/>
-      <c r="F71" s="83"/>
-      <c r="G71" s="83"/>
-      <c r="H71" s="83"/>
-      <c r="I71" s="83"/>
-      <c r="J71" s="83"/>
-      <c r="K71" s="83"/>
-      <c r="L71" s="83"/>
-      <c r="M71" s="83"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="83"/>
-      <c r="B72" s="83"/>
-      <c r="C72" s="83"/>
-      <c r="D72" s="83"/>
-      <c r="E72" s="83"/>
-      <c r="F72" s="83"/>
-      <c r="G72" s="83"/>
-      <c r="H72" s="83"/>
-      <c r="I72" s="83"/>
-      <c r="J72" s="83"/>
-      <c r="K72" s="83"/>
-      <c r="L72" s="83"/>
-      <c r="M72" s="83"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="83"/>
-      <c r="B73" s="83"/>
-      <c r="C73" s="83"/>
-      <c r="D73" s="83"/>
-      <c r="E73" s="83"/>
-      <c r="F73" s="83"/>
-      <c r="G73" s="83"/>
-      <c r="H73" s="83"/>
-      <c r="I73" s="83"/>
-      <c r="J73" s="83"/>
-      <c r="K73" s="83"/>
-      <c r="L73" s="83"/>
-      <c r="M73" s="83"/>
+      <c r="C45" s="83"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="60"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="78"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="59"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="60"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="78"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="59"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="60"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="78"/>
+      <c r="B48" s="59"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="60"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="78"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="60"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="78"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="60"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="78"/>
+      <c r="B51" s="59"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59"/>
+      <c r="F51" s="59"/>
+      <c r="G51" s="60"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="78"/>
+      <c r="B52" s="59"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
+      <c r="E52" s="59"/>
+      <c r="F52" s="59"/>
+      <c r="G52" s="60"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="78"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="60"/>
+    </row>
+    <row r="54" spans="1:7" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="84"/>
+      <c r="B54" s="75"/>
+      <c r="C54" s="75"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="75"/>
+      <c r="F54" s="75"/>
+      <c r="G54" s="76"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -2890,7 +2463,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ETML L,Normal"ETML&amp;C&amp;"-,Normal"Planification&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"-,Normal"&amp;D - GGZ&amp;C&amp;"-,Normal"&amp;F - &amp;A&amp;R&amp;"-,Normal"Page &amp;P/&amp;N</oddFooter>
@@ -2901,27 +2474,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet">
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning">
           <controlPr defaultSize="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:colOff>95250</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15365" r:id="rId5" name="btnCreateWorkSheet"/>
+        <control shapeId="15364" r:id="rId5" name="btnCreatePlanning"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2951,27 +2524,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning">
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>95250</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15364" r:id="rId9" name="btnCreatePlanning"/>
+        <control shapeId="15365" r:id="rId9" name="btnCreateWorkSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2989,10 +2562,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.5703125" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" style="29" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="29" customWidth="1"/>
-    <col min="4" max="16384" width="1.5703125" style="29"/>
+    <col min="1" max="1" width="17.85546875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="20" customWidth="1"/>
+    <col min="4" max="16384" width="1.5703125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3010,7 +2583,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="95" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -3019,24 +2592,14 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="97"/>
+      <c r="B4" s="96"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
-      <c r="D4" s="30"/>
-    </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-    </row>
-    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="20"/>
-    </row>
-    <row r="15" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="20"/>
+      <c r="D4" s="29"/>
     </row>
     <row r="16" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3094,7 +2657,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Feuil4"/>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -3102,11 +2665,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="87" style="29" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" style="29" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="29"/>
+    <col min="1" max="1" width="21.42578125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="87" style="20" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" style="20" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3117,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="17"/>
-      <c r="D1" s="87"/>
+      <c r="D1" s="85"/>
     </row>
     <row r="2" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -3133,61 +2696,61 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" s="53" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" s="52" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="11"/>
@@ -3210,179 +2773,113 @@
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="20"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="20"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="20"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="20"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="20"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="20"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="20"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="20"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="39"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="20"/>
-    </row>
-    <row r="31" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A31" s="41"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="20"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-    </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-    </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="30"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="35"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="35"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="36"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="38"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+    </row>
+    <row r="31" spans="1:8" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -3441,7 +2938,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Feuil8"/>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
@@ -3449,319 +2946,253 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="87" style="29" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" style="29" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="29"/>
+    <col min="1" max="1" width="21.42578125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="87" style="20" customWidth="1"/>
+    <col min="4" max="4" width="44.140625" style="20" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="44">
+      <c r="B1" s="43">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="54"/>
+      <c r="D1" s="53"/>
     </row>
     <row r="2" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
     </row>
-    <row r="5" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
     </row>
-    <row r="6" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
     </row>
-    <row r="7" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-    </row>
-    <row r="16" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-    </row>
-    <row r="17" spans="1:9" s="53" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+    </row>
+    <row r="16" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+    </row>
+    <row r="17" spans="1:8" s="52" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48" t="s">
+    <row r="18" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B18" s="47">
         <f>SUM(B3:B17)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-    </row>
-    <row r="19" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="50"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="20"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="36"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="20"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="20"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="20"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="20"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="20"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="20"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="20"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="20"/>
-    </row>
-    <row r="36" spans="1:9" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="41"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="20"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+    </row>
+    <row r="19" spans="1:8" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+    </row>
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="30"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="33"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="35"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="35"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="35"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="38"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+    </row>
+    <row r="36" spans="1:8" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -3820,497 +3251,455 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080FAF2F-C534-499F-8C25-95E6F074E70C}">
   <sheetPr codeName="Feuil9"/>
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:H153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" style="29" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="87" style="29" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" style="29" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="29"/>
+    <col min="1" max="1" width="21.42578125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="87" style="20" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" style="20" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="44">
+      <c r="B1" s="43">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="54">
+      <c r="D1" s="53">
         <f>Donnees!$C$9</f>
         <v>45894</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="53" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="52" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="90" t="s">
-        <v>48</v>
+      <c r="C3" s="88" t="s">
+        <v>47</v>
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" s="53" customFormat="1" ht="81" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="52" customFormat="1" ht="81" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="2">
         <v>4</v>
       </c>
-      <c r="C4" s="91" t="s">
-        <v>49</v>
+      <c r="C4" s="89" t="s">
+        <v>48</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="53" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="52" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="91" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="89" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="97" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="53" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="52" customFormat="1" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="91" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="10"/>
-    </row>
-    <row r="7" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="89" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
     </row>
-    <row r="8" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
     </row>
-    <row r="10" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
     </row>
-    <row r="11" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-    </row>
-    <row r="16" spans="1:4" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-    </row>
-    <row r="17" spans="1:9" s="53" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+    </row>
+    <row r="16" spans="1:4" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+    </row>
+    <row r="17" spans="1:8" s="52" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48" t="s">
+    <row r="18" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B18" s="47">
         <f>SUM(B3:B17)</f>
         <v>9</v>
       </c>
-      <c r="C18" s="89" t="s">
+      <c r="C18" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="49"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="50"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-    </row>
-    <row r="20" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="43" t="s">
+      <c r="D18" s="48"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+    </row>
+    <row r="20" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="44">
+      <c r="B20" s="43">
         <v>2</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="54">
+      <c r="D20" s="53">
         <f>$D$1+7</f>
         <v>45901</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="46" t="s">
+    <row r="21" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="4">
         <v>7</v>
       </c>
-      <c r="C22" s="90" t="s">
-        <v>47</v>
+      <c r="C22" s="88" t="s">
+        <v>46</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="54" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="54" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="2">
         <v>2</v>
       </c>
-      <c r="C23" s="91" t="s">
-        <v>52</v>
+      <c r="C23" s="89" t="s">
+        <v>51</v>
       </c>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="20"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="F25" s="31"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="20"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="34"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="20"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="20"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="20"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="20"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F30" s="36"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="20"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="20"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F32" s="36"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="20"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="51"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="20"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="51"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="52"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="20"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F33" s="36"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="50"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="50"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="41"/>
-      <c r="I36" s="20"/>
-    </row>
-    <row r="37" spans="1:9" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="48" t="s">
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+    </row>
+    <row r="37" spans="1:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="48">
+      <c r="B37" s="47">
         <f>SUM(B22:B36)</f>
         <v>9</v>
       </c>
-      <c r="C37" s="89" t="s">
+      <c r="C37" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-    </row>
-    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="50"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-    </row>
-    <row r="39" spans="1:9" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="43" t="s">
+      <c r="D37" s="48"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="49"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+    </row>
+    <row r="39" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="44">
+      <c r="B39" s="43">
         <v>3</v>
       </c>
-      <c r="C39" s="45" t="s">
+      <c r="C39" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="54">
+      <c r="D39" s="53">
         <f>$D$20+7</f>
         <v>45908</v>
       </c>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-    </row>
-    <row r="40" spans="1:9" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="46" t="s">
+    </row>
+    <row r="40" spans="1:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="46" t="s">
+      <c r="C40" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="46" t="s">
+      <c r="D40" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="4">
         <v>9</v>
       </c>
-      <c r="C41" s="90" t="s">
+      <c r="C41" s="88" t="s">
         <v>38</v>
       </c>
       <c r="D41" s="9"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="10"/>
@@ -4341,16 +3730,16 @@
       <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="51"/>
-      <c r="B53" s="51"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
+      <c r="A53" s="50"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="51"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="51"/>
-      <c r="B54" s="51"/>
-      <c r="C54" s="52"/>
-      <c r="D54" s="52"/>
+      <c r="A54" s="50"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
     </row>
     <row r="55" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
@@ -4359,50 +3748,50 @@
       <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="48" t="s">
+      <c r="A56" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B56" s="48">
+      <c r="B56" s="47">
         <f>SUM(B41:B55)</f>
         <v>9</v>
       </c>
-      <c r="C56" s="89" t="s">
+      <c r="C56" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D56" s="49"/>
+      <c r="D56" s="48"/>
     </row>
     <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="50"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
+      <c r="A57" s="49"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="49"/>
     </row>
     <row r="58" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B58" s="44">
+      <c r="B58" s="43">
         <v>4</v>
       </c>
-      <c r="C58" s="45" t="s">
+      <c r="C58" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D58" s="54">
+      <c r="D58" s="53">
         <f>$D$39+7</f>
         <v>45915</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="46" t="s">
+      <c r="A59" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="47" t="s">
+      <c r="B59" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="46" t="s">
+      <c r="C59" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="46" t="s">
+      <c r="D59" s="45" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4413,11 +3802,11 @@
       <c r="B60" s="4">
         <v>9</v>
       </c>
-      <c r="C60" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="D60" s="92" t="s">
-        <v>56</v>
+      <c r="C60" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" s="90" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4487,16 +3876,16 @@
       <c r="D71" s="10"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="51"/>
-      <c r="B72" s="51"/>
-      <c r="C72" s="52"/>
-      <c r="D72" s="52"/>
+      <c r="A72" s="50"/>
+      <c r="B72" s="50"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="51"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="51"/>
-      <c r="B73" s="51"/>
-      <c r="C73" s="52"/>
-      <c r="D73" s="52"/>
+      <c r="A73" s="50"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="51"/>
     </row>
     <row r="74" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
@@ -4505,50 +3894,50 @@
       <c r="D74" s="11"/>
     </row>
     <row r="75" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="48" t="s">
+      <c r="A75" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="48">
+      <c r="B75" s="47">
         <f>SUM(B60:B74)</f>
         <v>9</v>
       </c>
-      <c r="C75" s="89" t="s">
+      <c r="C75" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D75" s="49"/>
+      <c r="D75" s="48"/>
     </row>
     <row r="76" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="50"/>
-      <c r="B76" s="50"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50"/>
+      <c r="A76" s="49"/>
+      <c r="B76" s="49"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="49"/>
     </row>
     <row r="77" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="43" t="s">
+      <c r="A77" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B77" s="44">
+      <c r="B77" s="43">
         <v>5</v>
       </c>
-      <c r="C77" s="45" t="s">
+      <c r="C77" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D77" s="54">
+      <c r="D77" s="53">
         <f>$D$58+7</f>
         <v>45922</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="46" t="s">
+      <c r="A78" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="47" t="s">
+      <c r="B78" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="46" t="s">
+      <c r="C78" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D78" s="46" t="s">
+      <c r="D78" s="45" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4559,7 +3948,7 @@
       <c r="B79" s="4">
         <v>9</v>
       </c>
-      <c r="C79" s="90" t="s">
+      <c r="C79" s="88" t="s">
         <v>41</v>
       </c>
       <c r="D79" s="9"/>
@@ -4631,16 +4020,16 @@
       <c r="D90" s="10"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="51"/>
-      <c r="B91" s="51"/>
-      <c r="C91" s="52"/>
-      <c r="D91" s="52"/>
+      <c r="A91" s="50"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="51"/>
+      <c r="D91" s="51"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="51"/>
-      <c r="B92" s="51"/>
-      <c r="C92" s="52"/>
-      <c r="D92" s="52"/>
+      <c r="A92" s="50"/>
+      <c r="B92" s="50"/>
+      <c r="C92" s="51"/>
+      <c r="D92" s="51"/>
     </row>
     <row r="93" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
@@ -4649,78 +4038,78 @@
       <c r="D93" s="11"/>
     </row>
     <row r="94" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="48" t="s">
+      <c r="A94" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B94" s="48">
+      <c r="B94" s="47">
         <f>SUM(B79:B93)</f>
         <v>9</v>
       </c>
-      <c r="C94" s="89" t="s">
+      <c r="C94" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D94" s="49"/>
+      <c r="D94" s="48"/>
     </row>
     <row r="95" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="50"/>
-      <c r="B95" s="50"/>
-      <c r="C95" s="50"/>
-      <c r="D95" s="50"/>
+      <c r="A95" s="49"/>
+      <c r="B95" s="49"/>
+      <c r="C95" s="49"/>
+      <c r="D95" s="49"/>
     </row>
     <row r="96" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="43" t="s">
+      <c r="A96" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B96" s="44">
+      <c r="B96" s="43">
         <v>6</v>
       </c>
-      <c r="C96" s="45" t="s">
+      <c r="C96" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D96" s="54">
+      <c r="D96" s="53">
         <f>$D$77+7</f>
         <v>45929</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="46" t="s">
+      <c r="A97" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B97" s="47" t="s">
+      <c r="B97" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C97" s="46" t="s">
+      <c r="C97" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D97" s="46" t="s">
+      <c r="D97" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="77.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B98" s="4">
         <v>5</v>
       </c>
-      <c r="C98" s="90" t="s">
-        <v>54</v>
-      </c>
-      <c r="D98" s="93" t="s">
-        <v>44</v>
+      <c r="C98" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="D98" s="91" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B99" s="2">
         <v>4</v>
       </c>
-      <c r="C99" s="91" t="s">
-        <v>55</v>
-      </c>
-      <c r="D99" s="10"/>
+      <c r="C99" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="D99" s="97"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
@@ -4783,16 +4172,16 @@
       <c r="D109" s="10"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="51"/>
-      <c r="B110" s="51"/>
-      <c r="C110" s="52"/>
-      <c r="D110" s="52"/>
+      <c r="A110" s="50"/>
+      <c r="B110" s="50"/>
+      <c r="C110" s="51"/>
+      <c r="D110" s="51"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="51"/>
-      <c r="B111" s="51"/>
-      <c r="C111" s="52"/>
-      <c r="D111" s="52"/>
+      <c r="A111" s="50"/>
+      <c r="B111" s="50"/>
+      <c r="C111" s="51"/>
+      <c r="D111" s="51"/>
     </row>
     <row r="112" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
@@ -4801,50 +4190,50 @@
       <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="48" t="s">
+      <c r="A113" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B113" s="48">
+      <c r="B113" s="47">
         <f>SUM(B98:B112)</f>
         <v>9</v>
       </c>
-      <c r="C113" s="89" t="s">
+      <c r="C113" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D113" s="49"/>
+      <c r="D113" s="48"/>
     </row>
     <row r="114" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="50"/>
-      <c r="B114" s="50"/>
-      <c r="C114" s="50"/>
-      <c r="D114" s="50"/>
+      <c r="A114" s="49"/>
+      <c r="B114" s="49"/>
+      <c r="C114" s="49"/>
+      <c r="D114" s="49"/>
     </row>
     <row r="115" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="43" t="s">
+      <c r="A115" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B115" s="44">
+      <c r="B115" s="43">
         <v>7</v>
       </c>
-      <c r="C115" s="45" t="s">
+      <c r="C115" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D115" s="54">
+      <c r="D115" s="53">
         <f>$D$96+7</f>
         <v>45936</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="46" t="s">
+      <c r="A116" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B116" s="47" t="s">
+      <c r="B116" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C116" s="46" t="s">
+      <c r="C116" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D116" s="46" t="s">
+      <c r="D116" s="45" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4855,28 +4244,28 @@
       <c r="B117" s="4">
         <v>9</v>
       </c>
-      <c r="C117" s="90" t="s">
-        <v>46</v>
+      <c r="C117" s="88" t="s">
+        <v>45</v>
       </c>
       <c r="D117" s="9"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="2"/>
-      <c r="C118" s="98" t="s">
-        <v>57</v>
+      <c r="C118" s="92" t="s">
+        <v>56</v>
       </c>
       <c r="D118" s="10"/>
     </row>
     <row r="119" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B119" s="2">
         <v>6</v>
       </c>
-      <c r="C119" s="91" t="s">
-        <v>59</v>
+      <c r="C119" s="89" t="s">
+        <v>58</v>
       </c>
       <c r="D119" s="10"/>
     </row>
@@ -4935,16 +4324,16 @@
       <c r="D128" s="10"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="51"/>
-      <c r="B129" s="51"/>
-      <c r="C129" s="52"/>
-      <c r="D129" s="52"/>
+      <c r="A129" s="50"/>
+      <c r="B129" s="50"/>
+      <c r="C129" s="51"/>
+      <c r="D129" s="51"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="51"/>
-      <c r="B130" s="51"/>
-      <c r="C130" s="52"/>
-      <c r="D130" s="52"/>
+      <c r="A130" s="50"/>
+      <c r="B130" s="50"/>
+      <c r="C130" s="51"/>
+      <c r="D130" s="51"/>
     </row>
     <row r="131" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
@@ -4953,50 +4342,50 @@
       <c r="D131" s="11"/>
     </row>
     <row r="132" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="48" t="s">
+      <c r="A132" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B132" s="48">
+      <c r="B132" s="47">
         <f>SUM(B117:B131)</f>
         <v>15</v>
       </c>
-      <c r="C132" s="89" t="s">
-        <v>58</v>
-      </c>
-      <c r="D132" s="49"/>
+      <c r="C132" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="D132" s="48"/>
     </row>
     <row r="133" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="50"/>
-      <c r="B133" s="50"/>
-      <c r="C133" s="50"/>
-      <c r="D133" s="50"/>
+      <c r="A133" s="49"/>
+      <c r="B133" s="49"/>
+      <c r="C133" s="49"/>
+      <c r="D133" s="49"/>
     </row>
     <row r="134" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="43" t="s">
+      <c r="A134" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B134" s="44">
+      <c r="B134" s="43">
         <v>8</v>
       </c>
-      <c r="C134" s="45" t="s">
+      <c r="C134" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D134" s="54">
+      <c r="D134" s="53">
         <f>$D$115+7</f>
         <v>45943</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="46" t="s">
+      <c r="A135" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B135" s="47" t="s">
+      <c r="B135" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C135" s="46" t="s">
+      <c r="C135" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D135" s="46" t="s">
+      <c r="D135" s="45" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5073,16 +4462,16 @@
       <c r="D147" s="10"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="51"/>
-      <c r="B148" s="51"/>
-      <c r="C148" s="52"/>
-      <c r="D148" s="52"/>
+      <c r="A148" s="50"/>
+      <c r="B148" s="50"/>
+      <c r="C148" s="51"/>
+      <c r="D148" s="51"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="51"/>
-      <c r="B149" s="51"/>
-      <c r="C149" s="52"/>
-      <c r="D149" s="52"/>
+      <c r="A149" s="50"/>
+      <c r="B149" s="50"/>
+      <c r="C149" s="51"/>
+      <c r="D149" s="51"/>
     </row>
     <row r="150" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3"/>
@@ -5091,26 +4480,26 @@
       <c r="D150" s="11"/>
     </row>
     <row r="151" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="48" t="s">
+      <c r="A151" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B151" s="48">
+      <c r="B151" s="47">
         <f>SUM(B136:B150)</f>
         <v>0</v>
       </c>
-      <c r="C151" s="89" t="s">
+      <c r="C151" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D151" s="49"/>
+      <c r="D151" s="48"/>
     </row>
     <row r="152" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A152" s="50"/>
-      <c r="B152" s="50"/>
-      <c r="C152" s="50"/>
-      <c r="D152" s="50"/>
+      <c r="A152" s="49"/>
+      <c r="B152" s="49"/>
+      <c r="C152" s="49"/>
+      <c r="D152" s="49"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="88" t="s">
+      <c r="A153" s="86" t="s">
         <v>29</v>
       </c>
     </row>
@@ -5134,16 +4523,17 @@
   <hyperlinks>
     <hyperlink ref="D60" r:id="rId1" display="https://learn.microsoft.com/fr-fr/visualstudio/ide/create-csharp-winform-visual-studio?view=vs-2022 _x000a__x000a_chatgpt.com" xr:uid="{525590D3-AE3F-412E-AE63-77E2FB54C37E}"/>
     <hyperlink ref="D98" r:id="rId2" display="https://scottplot.net/" xr:uid="{96953D07-F238-4D18-B372-BC8B3B97A872}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{D13BD954-5271-41EB-873E-6E973D2530A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
+  <legacyDrawing r:id="rId6"/>
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="43009" r:id="rId6" name="btnImportRealisation">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="43009" r:id="rId7" name="btnImportRealisation">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -5162,7 +4552,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="43009" r:id="rId6" name="btnImportRealisation"/>
+        <control shapeId="43009" r:id="rId7" name="btnImportRealisation"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -5170,6 +4560,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Belge" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="14" ma:contentTypeDescription="Yeni belge oluşturun." ma:contentTypeScope="" ma:versionID="ee0afad02cec1cb5c008e069b7696935">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="071b3019c14a3acff1c11c5229ff0248" ns2:_="" ns3:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -5398,27 +4808,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15235525-7A96-4FDC-BE0C-FC0EC8076A2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5435,23 +4844,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C29126A-0525-4FCA-A870-5924A033DD5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{483719EA-391A-4C4B-985B-9805B7FCB9D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
doc(journal de travail): rédaction finale du journal de travail
</commit_message>
<xml_diff>
--- a/JDT/T-P_FUN-MatiasDenis-JDT.xlsx
+++ b/JDT/T-P_FUN-MatiasDenis-JDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\05-repertoires-ict-ssd (2022)\Deuxième année\P_FUN\P_FUN\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31D15B5-8D49-46D4-ACF4-AD6E792265BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD1B5EB-5826-4FD9-8AC3-671C00F9000E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Donnees" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
   <si>
     <t>Module :</t>
   </si>
@@ -272,6 +272,18 @@
 chatgpt.com
 https://learn.microsoft.com/fr-fr/visualstudio/ide/create-csharp-winform-visual-studio?view=vs-2022 
 https://chatgpt.com/c/68c7f767-915c-832b-bc1e-3d01b5980f03</t>
+  </si>
+  <si>
+    <t>Rédaction de la fin du rapport</t>
+  </si>
+  <si>
+    <t>Pendant les vacances</t>
+  </si>
+  <si>
+    <t>https://chatgpt.com/c/68c7f767-915c-832b-bc1e-3d01b5980f03</t>
+  </si>
+  <si>
+    <t>Rédaction du chapitre des tests fonctionnels grâce à ChatGPT pour gagner du temps avant le rendu.</t>
   </si>
 </sst>
 </file>
@@ -911,7 +923,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1176,6 +1188,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1186,7 +1202,11 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1559,7 +1579,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
-          <xdr:colOff>259080</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -2058,10 +2078,10 @@
     </row>
     <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78"/>
-      <c r="B19" s="93" t="s">
+      <c r="B19" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="94"/>
+      <c r="C19" s="95"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
@@ -2215,7 +2235,9 @@
       <c r="B31" s="79">
         <v>11</v>
       </c>
-      <c r="C31" s="70"/>
+      <c r="C31" s="70" t="s">
+        <v>60</v>
+      </c>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
       <c r="F31" s="59"/>
@@ -2463,7 +2485,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="57" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="52" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ETML L,Normal"ETML&amp;C&amp;"-,Normal"Planification&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;"-,Normal"&amp;D - GGZ&amp;C&amp;"-,Normal"&amp;F - &amp;A&amp;R&amp;"-,Normal"Page &amp;P/&amp;N</oddFooter>
@@ -2583,7 +2605,7 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="96" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="16">
@@ -2592,7 +2614,7 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="96"/>
+      <c r="B4" s="97"/>
       <c r="C4" s="22">
         <v>0</v>
       </c>
@@ -3253,8 +3275,8 @@
   <sheetPr codeName="Feuil9"/>
   <dimension ref="A1:H153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="K137" sqref="K137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3331,7 +3353,7 @@
       <c r="C5" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="93" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4109,7 +4131,7 @@
       <c r="C99" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="D99" s="97"/>
+      <c r="D99" s="93"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
@@ -4267,7 +4289,7 @@
       <c r="C119" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="D119" s="10"/>
+      <c r="D119" s="93"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
@@ -4392,14 +4414,24 @@
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="4"/>
-      <c r="C136" s="9"/>
+      <c r="C136" s="98" t="s">
+        <v>61</v>
+      </c>
       <c r="D136" s="9"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
+    <row r="137" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B137" s="2">
+        <v>9</v>
+      </c>
+      <c r="C137" s="99" t="s">
+        <v>63</v>
+      </c>
+      <c r="D137" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
@@ -4485,7 +4517,7 @@
       </c>
       <c r="B151" s="47">
         <f>SUM(B136:B150)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C151" s="87" t="s">
         <v>28</v>

</xml_diff>